<commit_message>
Incremental fitness update bug found, Settings, Timer
</commit_message>
<xml_diff>
--- a/res/benchmarks.xlsx
+++ b/res/benchmarks.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="363235653CEFB026356243E929449944C10C528E" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="363235653CEFB026356243E929449944C10C528E" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -756,7 +756,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Delta fitness criteria improved (using moving average)
</commit_message>
<xml_diff>
--- a/res/benchmarks.xlsx
+++ b/res/benchmarks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="363235653CEFB026356243E929449944C10C528E" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="363235653CEFB026356243E929449944C10C528E" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{24C09E9C-E816-496C-861D-D22B94736A14}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -756,7 +756,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,10 +835,12 @@
       <c r="G4" s="9">
         <v>157.03273300000001</v>
       </c>
-      <c r="I4" s="23"/>
+      <c r="I4" s="23">
+        <v>180.97507999999999</v>
+      </c>
       <c r="J4" s="24">
         <f>100*(I4-G4)/G4</f>
-        <v>-100</v>
+        <v>15.246723751537827</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -975,10 +977,12 @@
       <c r="G9" s="10">
         <v>3.044578</v>
       </c>
-      <c r="I9" s="22"/>
+      <c r="I9" s="22">
+        <v>4.9803796</v>
+      </c>
       <c r="J9" s="3">
         <f t="shared" si="0"/>
-        <v>-100</v>
+        <v>63.5819348362893</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1024,7 +1028,7 @@
       </c>
       <c r="J13" s="4">
         <f>AVERAGE(J4:J10)</f>
-        <v>-100</v>
+        <v>-60.167334487453267</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1033,7 +1037,7 @@
       </c>
       <c r="J14" s="4">
         <f>MAX(J4:J10)</f>
-        <v>-99.999999999999986</v>
+        <v>63.5819348362893</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Settings used for final release
</commit_message>
<xml_diff>
--- a/res/benchmarks.xlsx
+++ b/res/benchmarks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="3" documentId="363235653CEFB026356243E929449944C10C528E" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{24C09E9C-E816-496C-861D-D22B94736A14}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="363235653CEFB026356243E929449944C10C528E" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{5F106A41-7E78-43C5-9963-000ECF3C3B07}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -756,7 +756,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,11 +836,11 @@
         <v>157.03273300000001</v>
       </c>
       <c r="I4" s="23">
-        <v>180.97507999999999</v>
+        <v>180.97476</v>
       </c>
       <c r="J4" s="24">
         <f>100*(I4-G4)/G4</f>
-        <v>15.246723751537827</v>
+        <v>15.246519972367798</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -865,10 +865,12 @@
       <c r="G5" s="10">
         <v>34.708820000000003</v>
       </c>
-      <c r="I5" s="22"/>
+      <c r="I5" s="22">
+        <v>46.11374</v>
+      </c>
       <c r="J5" s="3">
         <f t="shared" ref="J5:J10" si="0">100*(I5-G5)/G5</f>
-        <v>-100</v>
+        <v>32.858852591358612</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -893,10 +895,12 @@
       <c r="G6" s="10">
         <v>32.626666999999998</v>
       </c>
-      <c r="I6" s="22"/>
+      <c r="I6" s="22">
+        <v>47.678894</v>
+      </c>
       <c r="J6" s="3">
         <f t="shared" si="0"/>
-        <v>-100</v>
+        <v>46.13473696225239</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -921,10 +925,12 @@
       <c r="G7" s="10">
         <v>7.7172020000000003</v>
       </c>
-      <c r="I7" s="22"/>
+      <c r="I7" s="22">
+        <v>10.917183</v>
+      </c>
       <c r="J7" s="3">
         <f t="shared" si="0"/>
-        <v>-99.999999999999986</v>
+        <v>41.46555966786925</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -949,10 +955,12 @@
       <c r="G8" s="10">
         <v>12.901103000000001</v>
       </c>
-      <c r="I8" s="22"/>
+      <c r="I8" s="22">
+        <v>18.962624000000002</v>
+      </c>
       <c r="J8" s="3">
         <f t="shared" si="0"/>
-        <v>-100</v>
+        <v>46.984517525361987</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -978,11 +986,11 @@
         <v>3.044578</v>
       </c>
       <c r="I9" s="22">
-        <v>4.9803796</v>
+        <v>4.4145764999999999</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" si="0"/>
-        <v>63.5819348362893</v>
+        <v>44.997976731093758</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1007,10 +1015,12 @@
       <c r="G10" s="12">
         <v>10.050300999999999</v>
       </c>
-      <c r="I10" s="22"/>
+      <c r="I10" s="22">
+        <v>14.834254</v>
+      </c>
       <c r="J10" s="3">
         <f t="shared" si="0"/>
-        <v>-100</v>
+        <v>47.600096753321125</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1019,7 +1029,7 @@
       </c>
       <c r="J12" s="4">
         <f>MIN(J4:J10)</f>
-        <v>-100</v>
+        <v>15.246519972367798</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1028,7 +1038,7 @@
       </c>
       <c r="J13" s="4">
         <f>AVERAGE(J4:J10)</f>
-        <v>-60.167334487453267</v>
+        <v>39.32689431480356</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1037,7 +1047,7 @@
       </c>
       <c r="J14" s="4">
         <f>MAX(J4:J10)</f>
-        <v>63.5819348362893</v>
+        <v>47.600096753321125</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1054,7 +1064,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>